<commit_message>
Testdata correction due to LIVEHTA-1269
</commit_message>
<xml_diff>
--- a/Testdata/Non_Oncology/DataFiles/Protocol_Page/PRISMA/PRISMA_Nononco_Data.xlsx
+++ b/Testdata/Non_Oncology/DataFiles/Protocol_Page/PRISMA/PRISMA_Nononco_Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\Non_Oncology\DataFiles\Protocol_Page\PRISMA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9BAD6CB-6AE9-4092-820B-863A4AC9B8FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC49863F-661D-47B9-A0D3-80925218391C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
   <si>
     <t>Economic</t>
   </si>
@@ -55,18 +55,6 @@
     <t>Prisma_Image</t>
   </si>
   <si>
-    <t>OriginalStudiesNumbers</t>
-  </si>
-  <si>
-    <t>RecordsNumber</t>
-  </si>
-  <si>
-    <t>fullTextReviewRecordsNumber</t>
-  </si>
-  <si>
-    <t>totalRecordsNumber</t>
-  </si>
-  <si>
     <t>Prisma_Population</t>
   </si>
   <si>
@@ -95,6 +83,42 @@
   </si>
   <si>
     <t>Clinical-RWE</t>
+  </si>
+  <si>
+    <t>stdy_type_locators</t>
+  </si>
+  <si>
+    <t>total_record_number</t>
+  </si>
+  <si>
+    <t>total_excluded_number</t>
+  </si>
+  <si>
+    <t>total_screenedTiAb_number</t>
+  </si>
+  <si>
+    <t>total_excluded_screenedTiAb_number</t>
+  </si>
+  <si>
+    <t>fulltext_review</t>
+  </si>
+  <si>
+    <t>excluded_fulltext_review</t>
+  </si>
+  <si>
+    <t>fulltext_exclusion_reason</t>
+  </si>
+  <si>
+    <t>total_greyliterature_number</t>
+  </si>
+  <si>
+    <t>original_studies</t>
+  </si>
+  <si>
+    <t>records_number</t>
+  </si>
+  <si>
+    <t>stdy_type_values</t>
   </si>
 </sst>
 </file>
@@ -421,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -433,19 +457,17 @@
     <col min="2" max="2" width="28.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="67.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="71.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="71.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
@@ -454,140 +476,159 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2">
+        <v>100</v>
+      </c>
+      <c r="G2" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E3" t="s">
         <v>18</v>
       </c>
-      <c r="E2">
-        <v>500</v>
-      </c>
-      <c r="F2">
-        <v>1000</v>
-      </c>
-      <c r="G2">
-        <v>1500</v>
-      </c>
-      <c r="H2">
-        <v>2000</v>
-      </c>
-      <c r="I2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3">
-        <v>600</v>
-      </c>
       <c r="F3">
-        <v>1200</v>
-      </c>
-      <c r="G3">
-        <v>1800</v>
-      </c>
-      <c r="H3">
-        <v>2400</v>
-      </c>
-      <c r="I3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
       </c>
-      <c r="E4">
-        <v>700</v>
+      <c r="E4" t="s">
+        <v>19</v>
       </c>
       <c r="F4">
-        <v>1400</v>
-      </c>
-      <c r="G4">
-        <v>2100</v>
-      </c>
-      <c r="H4">
-        <v>2800</v>
-      </c>
-      <c r="I4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <v>300</v>
+      </c>
+      <c r="G4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
         <v>1</v>
       </c>
-      <c r="E5">
-        <v>800</v>
+      <c r="E5" t="s">
+        <v>20</v>
       </c>
       <c r="F5">
-        <v>1600</v>
-      </c>
-      <c r="G5">
-        <v>2400</v>
-      </c>
-      <c r="H5">
-        <v>3200</v>
-      </c>
-      <c r="I5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>400</v>
+      </c>
+      <c r="G5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
         <v>2</v>
       </c>
-      <c r="E6">
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6">
+        <v>500</v>
+      </c>
+      <c r="G6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10">
         <v>900</v>
       </c>
-      <c r="F6">
-        <v>1800</v>
-      </c>
-      <c r="G6">
-        <v>2700</v>
-      </c>
-      <c r="H6">
-        <v>3600</v>
-      </c>
-      <c r="I6" t="s">
-        <v>11</v>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the missed validation
</commit_message>
<xml_diff>
--- a/Testdata/Non_Oncology/DataFiles/Protocol_Page/PRISMA/PRISMA_Nononco_Data.xlsx
+++ b/Testdata/Non_Oncology/DataFiles/Protocol_Page/PRISMA/PRISMA_Nononco_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\Non_Oncology\DataFiles\Protocol_Page\PRISMA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B878F4A-4091-487E-8B53-57AEB244E787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C6192E-F9DC-49E5-ADB8-9D75CC83F61C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="49">
   <si>
     <t>Study_Types</t>
   </si>
@@ -149,6 +149,39 @@
   </si>
   <si>
     <t>*This field is required.</t>
+  </si>
+  <si>
+    <t>pop3</t>
+  </si>
+  <si>
+    <t>text1</t>
+  </si>
+  <si>
+    <t>text2</t>
+  </si>
+  <si>
+    <t>text3</t>
+  </si>
+  <si>
+    <t>text4</t>
+  </si>
+  <si>
+    <t>text5</t>
+  </si>
+  <si>
+    <t>text6</t>
+  </si>
+  <si>
+    <t>text7</t>
+  </si>
+  <si>
+    <t>text8</t>
+  </si>
+  <si>
+    <t>text9</t>
+  </si>
+  <si>
+    <t>*This field must be digits</t>
   </si>
 </sst>
 </file>
@@ -475,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="E8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L24" sqref="F24:L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -817,6 +850,156 @@
         <v>36</v>
       </c>
     </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" t="s">
+        <v>39</v>
+      </c>
+      <c r="G24" t="s">
+        <v>25</v>
+      </c>
+      <c r="H24" t="s">
+        <v>26</v>
+      </c>
+      <c r="L24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" t="s">
+        <v>40</v>
+      </c>
+      <c r="G25" t="s">
+        <v>25</v>
+      </c>
+      <c r="H25" t="s">
+        <v>26</v>
+      </c>
+      <c r="L25" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>38</v>
+      </c>
+      <c r="E26" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" t="s">
+        <v>41</v>
+      </c>
+      <c r="L26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" t="s">
+        <v>42</v>
+      </c>
+      <c r="L27" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" t="s">
+        <v>43</v>
+      </c>
+      <c r="L28" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>38</v>
+      </c>
+      <c r="E29" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" t="s">
+        <v>44</v>
+      </c>
+      <c r="L29" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30" t="s">
+        <v>45</v>
+      </c>
+      <c r="L30" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>38</v>
+      </c>
+      <c r="E31" t="s">
+        <v>16</v>
+      </c>
+      <c r="F31" t="s">
+        <v>46</v>
+      </c>
+      <c r="L31" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>38</v>
+      </c>
+      <c r="E32" t="s">
+        <v>17</v>
+      </c>
+      <c r="F32" t="s">
+        <v>47</v>
+      </c>
+      <c r="L32" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>